<commit_message>
Fixed unconnected symbol on schematics. Generated new PDF schematics. Fixed BoM and PnP files for JLCPB assembly.
</commit_message>
<xml_diff>
--- a/cam/Uno_v1.0_2021-04-14-BoM.xlsx
+++ b/cam/Uno_v1.0_2021-04-14-BoM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\Uno\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2DF41D-BE6B-4BA5-8332-5AE17EE933F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E03C52E-77C1-4C4D-BF2A-94EF80D8A485}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17040" yWindow="430" windowWidth="16430" windowHeight="19950" xr2:uid="{0C47F62E-93AD-4038-96AB-D6C8EFD49D8B}"/>
+    <workbookView xWindow="1430" yWindow="400" windowWidth="16430" windowHeight="19950" xr2:uid="{0C47F62E-93AD-4038-96AB-D6C8EFD49D8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -335,9 +335,6 @@
     <t>SOIC-8_3.9x4.9x1.27P</t>
   </si>
   <si>
-    <t>C7377</t>
-  </si>
-  <si>
     <t>LM358DR2G</t>
   </si>
   <si>
@@ -351,6 +348,9 @@
   </si>
   <si>
     <t>4</t>
+  </si>
+  <si>
+    <t>C1017</t>
   </si>
 </sst>
 </file>
@@ -813,7 +813,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1019,13 +1019,13 @@
         <v>98</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="F10" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -1042,7 +1042,7 @@
         <v>51</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>53</v>
@@ -1210,10 +1210,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>65</v>
@@ -1351,10 +1351,10 @@
     <hyperlink ref="E13" r:id="rId18" display="https://lcsc.com/product-detail/Light-Emitting-Diodes-LED_0603-Blue-light_C72041.html/?href=jlc-SMT" xr:uid="{837492DF-9729-4BD2-8EB6-328EF51BAAC1}"/>
     <hyperlink ref="E12" r:id="rId19" display="https://lcsc.com/product-detail/Light-Emitting-Diodes-LED_0603-Green-light_C72043.html/?href=jlc-SMT" xr:uid="{DC4DF417-ABF9-45EB-AF24-D930584C6A1E}"/>
     <hyperlink ref="E14" r:id="rId20" display="https://lcsc.com/product-detail/Light-Emitting-Diodes-LED_0603-Yellow-light_C72038.html/?href=jlc-SMT" xr:uid="{C121B20F-28BF-4B04-B551-2F773F754B0D}"/>
-    <hyperlink ref="E11" r:id="rId21" display="https://lcsc.com/product-detail/Beads_Sunlord-GZ2012D601TF_C1017.html/?href=jlc-SMT" xr:uid="{B984933C-C0DC-4EC3-B525-1020A92FACAF}"/>
-    <hyperlink ref="E24" r:id="rId22" display="https://lcsc.com/product-detail/USB_CH340G_C14267.html/?href=jlc-SMT" xr:uid="{D3ACCC8A-1694-4E7C-9C7C-9296DCE3F76D}"/>
-    <hyperlink ref="E6" r:id="rId23" display="https://lcsc.com/product-detail/Diodes-General-Purpose_MDD-Microdiode-Electronics-MDD-Jiangsu-Yutai-Elec-M7-GPP_C95872.html/?href=jlc-SMT" xr:uid="{C030F1FE-0D2C-48E3-B159-AE900057C1B4}"/>
-    <hyperlink ref="E10" r:id="rId24" display="https://lcsc.com/product-detail/Low-Power-OpAmps_MICROCHIP_MCP6002T-I-SN_MCP6002T-I-SN_C7377.html/?href=jlc-SMT" xr:uid="{F91D3485-B91F-4761-94CA-66BB9606845B}"/>
+    <hyperlink ref="E24" r:id="rId21" display="https://lcsc.com/product-detail/USB_CH340G_C14267.html/?href=jlc-SMT" xr:uid="{D3ACCC8A-1694-4E7C-9C7C-9296DCE3F76D}"/>
+    <hyperlink ref="E6" r:id="rId22" display="https://lcsc.com/product-detail/Diodes-General-Purpose_MDD-Microdiode-Electronics-MDD-Jiangsu-Yutai-Elec-M7-GPP_C95872.html/?href=jlc-SMT" xr:uid="{C030F1FE-0D2C-48E3-B159-AE900057C1B4}"/>
+    <hyperlink ref="E11" r:id="rId23" display="https://lcsc.com/product-detail/Beads_Sunlord-GZ2012D601TF_C1017.html/?href=jlc-SMT" xr:uid="{085B36C3-EFA3-430B-A6F9-78CCB44D0708}"/>
+    <hyperlink ref="E10" r:id="rId24" display="https://lcsc.com/product-detail/General-Purpose-Amplifiers_ON-Semicon_LM358DR2G_ON-Semicon-ON-LM358DR2G_C7950.html/?href=jlc-SMT" xr:uid="{045119BB-51F8-40CF-B8C2-2153A4AC9640}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId25"/>

</xml_diff>